<commit_message>
Deploying to gh-pages from  @ 5c525fcd598dad490d44a219ce8c28a5c7c6374c 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.1.1.xlsx
+++ b/en/downloads/data-excel/3.1.1.xlsx
@@ -738,11 +738,13 @@
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="39.28515625" customWidth="1"/>
+    <col min="1" max="3" width="34.42578125" customWidth="1"/>
     <col min="4" max="14" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -903,7 +905,7 @@
         <v>31.896888425986198</v>
       </c>
       <c r="O5" s="23">
-        <v>24.5</v>
+        <v>28.6</v>
       </c>
       <c r="P5" s="23">
         <v>24.8</v>
@@ -953,7 +955,7 @@
         <v>51.944197091124963</v>
       </c>
       <c r="O6" s="24">
-        <v>20.2</v>
+        <v>33.6</v>
       </c>
       <c r="P6" s="24">
         <v>25.8</v>
@@ -1053,7 +1055,7 @@
         <v>36.95491500369549</v>
       </c>
       <c r="O8" s="24">
-        <v>53.4</v>
+        <v>71.2</v>
       </c>
       <c r="P8" s="24">
         <v>28.4</v>
@@ -1253,7 +1255,7 @@
         <v>22.949465277459037</v>
       </c>
       <c r="O12" s="24">
-        <v>4</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="P12" s="24">
         <v>32.5</v>

</xml_diff>